<commit_message>
updated extension to automatically install required programs on Windows, macos, and Linux
</commit_message>
<xml_diff>
--- a/board/esp32-current/bom/bom.xlsx
+++ b/board/esp32-current/bom/bom.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\School\TTU\summer23\project-lab-4\iCEGenius\board\bom\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\School\TTU\summer23\project-lab-4\iCEGenius\board\esp32-current\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB001C92-EE87-4061-B437-4DF7468594B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{849D7608-E3C5-4FF0-A241-578696C7F99D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="20832" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="v2" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="92">
   <si>
     <t>Part Name</t>
   </si>
@@ -216,21 +216,6 @@
     <t>Price</t>
   </si>
   <si>
-    <t>ASFL1-100.000MHZ-L-T</t>
-  </si>
-  <si>
-    <t>815-ASFL1-100-L-T</t>
-  </si>
-  <si>
-    <t>100MHz Clock</t>
-  </si>
-  <si>
-    <t>MCP2210-I_MQ</t>
-  </si>
-  <si>
-    <t>579-MCP2210IMQ</t>
-  </si>
-  <si>
     <t>Amount/Unit</t>
   </si>
   <si>
@@ -249,15 +234,6 @@
     <t>0.01n X7R 10% 0201 10% Cap</t>
   </si>
   <si>
-    <t>MMBT3904-TP</t>
-  </si>
-  <si>
-    <t>833-MMBT3904-TP</t>
-  </si>
-  <si>
-    <t>NPN BJT</t>
-  </si>
-  <si>
     <t>576-SC1006-01LTG</t>
   </si>
   <si>
@@ -282,16 +258,67 @@
     <t>Savings from v1</t>
   </si>
   <si>
-    <t>755-BU33SD5WG-TR</t>
-  </si>
-  <si>
-    <t>BU33SD5WG-TR</t>
+    <t xml:space="preserve">595-ESD321DYAR </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESD321DYAR </t>
+  </si>
+  <si>
+    <t>579-MCP1727-3302E/MF</t>
+  </si>
+  <si>
+    <t>MCP1727-3302E/MF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">520-TXO32CSMV400BNTR </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECS-TXO-32CSMV-400-BN-TR </t>
+  </si>
+  <si>
+    <t>40MHz TCXO</t>
+  </si>
+  <si>
+    <t>998-PL133-27GC-R</t>
+  </si>
+  <si>
+    <t>PL133-27GC-R</t>
+  </si>
+  <si>
+    <t>Clock 1:2 Buffer</t>
+  </si>
+  <si>
+    <t>356-ESP32-C6FH4</t>
+  </si>
+  <si>
+    <t>ESP32-C6FH4</t>
+  </si>
+  <si>
+    <t>10u X5R 0402 20% Cap</t>
+  </si>
+  <si>
+    <t>81-GRM155R61A106ME1J</t>
+  </si>
+  <si>
+    <t>GRM155R61A106ME11J</t>
+  </si>
+  <si>
+    <t xml:space="preserve">81-LQG15HZ2N0B02D </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LQG15HZ2N0B02D </t>
+  </si>
+  <si>
+    <t>2n 0.9A Inductor</t>
+  </si>
+  <si>
+    <t>100n X5R 0201 10% Cap</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -354,7 +381,9 @@
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{5C37FC90-03B5-4C0A-8076-F8209C1FD0BE}"/>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -630,25 +659,25 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B12B033B-7B25-49A8-990D-BD5EF448ABF6}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.90625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="11.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>37</v>
       </c>
@@ -659,7 +688,7 @@
         <v>58</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
@@ -668,13 +697,13 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -682,27 +711,27 @@
         <v>2</v>
       </c>
       <c r="C2" s="2">
-        <v>2.17</v>
+        <v>2.2799999999999998</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" s="2">
         <f t="shared" ref="E2:E20" si="0">C2*D2</f>
-        <v>2.17</v>
+        <v>2.2799999999999998</v>
       </c>
       <c r="F2" t="s">
         <v>5</v>
       </c>
       <c r="G2" s="3">
         <f>G5*H2</f>
-        <v>39.689999999999991</v>
+        <v>13.44</v>
       </c>
       <c r="H2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>57</v>
       </c>
@@ -710,44 +739,44 @@
         <v>3</v>
       </c>
       <c r="C3" s="2">
-        <v>0.52</v>
+        <v>0.49</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" s="2">
         <f t="shared" si="0"/>
-        <v>0.52</v>
+        <v>0.49</v>
       </c>
       <c r="F3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B4" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C4" s="2">
-        <v>0.6</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" s="2">
         <f t="shared" si="0"/>
-        <v>0.6</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="F4" t="s">
         <v>8</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>54</v>
       </c>
@@ -769,10 +798,10 @@
       </c>
       <c r="G5" s="2">
         <f>SUM(E2:E37)</f>
-        <v>13.229999999999997</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+        <v>13.44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>53</v>
       </c>
@@ -780,90 +809,90 @@
         <v>36</v>
       </c>
       <c r="C6" s="2">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="E6" s="2">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
       <c r="F6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>77</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>78</v>
       </c>
       <c r="C7" s="2">
-        <v>0.72</v>
+        <v>1.93</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7" s="2">
         <f t="shared" si="0"/>
-        <v>0.72</v>
+        <v>1.93</v>
       </c>
       <c r="F7" t="s">
-        <v>14</v>
+        <v>79</v>
       </c>
       <c r="G7" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>60</v>
-      </c>
       <c r="B8" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="C8" s="2">
-        <v>1.75</v>
+        <v>0.97</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8" s="2">
         <f t="shared" si="0"/>
-        <v>1.75</v>
+        <v>0.97</v>
       </c>
       <c r="F8" t="s">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="G8" s="4">
         <f>1-(G5/'v1'!G2)</f>
-        <v>6.9620253164557111E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+        <v>5.4852320675105481E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="B9" t="s">
-        <v>62</v>
+        <v>84</v>
       </c>
       <c r="C9" s="2">
-        <v>2.83</v>
+        <v>2.06</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
       <c r="E9" s="2">
         <f t="shared" si="0"/>
-        <v>2.83</v>
+        <v>2.06</v>
       </c>
       <c r="F9" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -874,38 +903,38 @@
         <v>0.04</v>
       </c>
       <c r="D10">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E10" s="2">
         <f t="shared" si="0"/>
-        <v>0.48</v>
+        <v>0.52</v>
       </c>
       <c r="F10" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>86</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>87</v>
       </c>
       <c r="C11" s="2">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
       <c r="D11">
         <v>2</v>
       </c>
       <c r="E11" s="2">
         <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>0.22</v>
       </c>
       <c r="F11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>47</v>
       </c>
@@ -916,17 +945,17 @@
         <v>0.02</v>
       </c>
       <c r="D12">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E12" s="2">
         <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="F12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>46</v>
       </c>
@@ -947,7 +976,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>44</v>
       </c>
@@ -958,38 +987,38 @@
         <v>0.08</v>
       </c>
       <c r="D14">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E14" s="2">
         <f t="shared" si="0"/>
-        <v>0.64</v>
+        <v>0.48</v>
       </c>
       <c r="F14" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>43</v>
+        <v>88</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>89</v>
       </c>
       <c r="C15" s="2">
-        <v>0.1</v>
+        <v>0.17</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
       <c r="E15" s="2">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>0.17</v>
       </c>
       <c r="F15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -1010,7 +1039,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>41</v>
       </c>
@@ -1031,12 +1060,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B18" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C18" s="2">
         <v>0.12</v>
@@ -1049,49 +1078,28 @@
         <v>0.12</v>
       </c>
       <c r="F18" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B19" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C19" s="2">
-        <v>0.1</v>
+        <v>0.45</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E19" s="2">
-        <f t="shared" si="0"/>
-        <v>0.1</v>
+        <f>C19*D19</f>
+        <v>1.35</v>
       </c>
       <c r="F19" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>73</v>
-      </c>
-      <c r="B20" t="s">
-        <v>74</v>
-      </c>
-      <c r="C20" s="2">
-        <v>0.45</v>
-      </c>
-      <c r="D20">
-        <v>3</v>
-      </c>
-      <c r="E20" s="2">
-        <f t="shared" si="0"/>
-        <v>1.35</v>
-      </c>
-      <c r="F20" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1109,19 +1117,19 @@
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>37</v>
       </c>
@@ -1132,7 +1140,7 @@
         <v>58</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
@@ -1141,11 +1149,11 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -1171,7 +1179,7 @@
       </c>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>57</v>
       </c>
@@ -1192,7 +1200,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>56</v>
       </c>
@@ -1213,7 +1221,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>55</v>
       </c>
@@ -1234,7 +1242,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>54</v>
       </c>
@@ -1255,7 +1263,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>53</v>
       </c>
@@ -1276,7 +1284,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1297,7 +1305,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>51</v>
       </c>
@@ -1318,7 +1326,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -1339,7 +1347,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -1360,7 +1368,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>48</v>
       </c>
@@ -1381,7 +1389,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>47</v>
       </c>
@@ -1402,7 +1410,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>46</v>
       </c>
@@ -1423,7 +1431,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>45</v>
       </c>
@@ -1444,7 +1452,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>44</v>
       </c>
@@ -1465,7 +1473,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -1486,7 +1494,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>42</v>
       </c>
@@ -1507,7 +1515,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>41</v>
       </c>
@@ -1528,12 +1536,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="B20" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C20" s="2">
         <v>0.45</v>
@@ -1546,12 +1554,12 @@
         <v>1.35</v>
       </c>
       <c r="F20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="C21" s="2">
         <v>1.87</v>
@@ -1564,7 +1572,7 @@
         <v>1.87</v>
       </c>
       <c r="F21" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>